<commit_message>
message list added, import attribute creation added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Event.xlsx
+++ b/src/test/resources/testData/Event.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>SKU</t>
   </si>
@@ -23,6 +23,21 @@
     <t>Family</t>
   </si>
   <si>
+    <t>isTestEvent</t>
+  </si>
+  <si>
+    <t>NewBoolean</t>
+  </si>
+  <si>
+    <t>NewText</t>
+  </si>
+  <si>
+    <t>NewSelect</t>
+  </si>
+  <si>
+    <t>NewDate</t>
+  </si>
+  <si>
     <t>City_Roof</t>
   </si>
   <si>
@@ -53,40 +68,61 @@
     <t>Etkinlik Adı</t>
   </si>
   <si>
-    <t>bbc7f7be-79a1-4019-b55d-9397b898c962</t>
+    <t>f1c3baaa-c96d-4166-bcda-7d30f7257f16</t>
   </si>
   <si>
     <t>Kurumsal İletişim</t>
   </si>
   <si>
-    <t>eb243df2-1f8a-468d-ac30-88c9ea39cbe3</t>
+    <t>TestAutomation</t>
+  </si>
+  <si>
+    <t>Option1</t>
+  </si>
+  <si>
+    <t>a4c9f46e-df05-49ce-81d8-2ec5946fb3af</t>
   </si>
   <si>
     <t>ROOT</t>
   </si>
   <si>
-    <t>f482dae0-b648-4b37-a335-30d08428e9cf</t>
+    <t>18.02.2026</t>
+  </si>
+  <si>
+    <t>Doğru</t>
+  </si>
+  <si>
+    <t>Option2</t>
+  </si>
+  <si>
+    <t>56815bb8-bb1c-4186-bb9a-fb87d0bb9d56</t>
   </si>
   <si>
     <t>Tümü</t>
   </si>
   <si>
-    <t>fae53ac6-bf85-4c6f-8db9-b8ec3469791e</t>
-  </si>
-  <si>
-    <t>a6a7cf24-80e7-46ea-9bf3-a957b6860f0c</t>
+    <t>ad7bf66c-1029-4e7b-9688-e290195e2856</t>
+  </si>
+  <si>
+    <t>Yanlış</t>
+  </si>
+  <si>
+    <t>Option3</t>
+  </si>
+  <si>
+    <t>838bef50-fdfd-4dbd-8ef4-62623599c933</t>
+  </si>
+  <si>
+    <t>Konferans</t>
   </si>
   <si>
     <t>Event-04</t>
   </si>
   <si>
-    <t>76b45333-5007-46db-86d0-f45ef9549411</t>
-  </si>
-  <si>
-    <t>Konferans</t>
-  </si>
-  <si>
-    <t>Hayır</t>
+    <t>0e409ae9-0cb2-4b19-bf1a-3d4282e882e3</t>
+  </si>
+  <si>
+    <t>16.02.2026</t>
   </si>
   <si>
     <t>Event-08</t>
@@ -99,7 +135,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd.MM.yyyy"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11.0"/>
@@ -129,15 +167,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -163,7 +204,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s" s="0">
         <v>7</v>
@@ -178,81 +219,123 @@
         <v>10</v>
       </c>
       <c r="L1" t="s" s="0">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="M1" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s" s="0">
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H3" t="n" s="1">
+        <v>46071.0</v>
       </c>
     </row>
     <row r="4">
       <c r="C4" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s" s="0">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>30</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>19</v>
+        <v>31</v>
+      </c>
+      <c r="L5" t="s" s="0">
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="P6" t="s" s="0">
+        <v>33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="K7" t="s" s="0">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="N7" t="n" s="2">
+        <v>46071.0</v>
+      </c>
+      <c r="O7" t="n" s="3">
+        <v>46069.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="L8" t="s" s="0">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>